<commit_message>
Oct 11 06:54 - Updated kode kloud
Added kode kloud credentials
</commit_message>
<xml_diff>
--- a/70lpa.xlsx
+++ b/70lpa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishin.pradeep\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EC94DD-B5B0-40CE-BE04-C2E679B15E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775AF131-49FB-4499-A9A1-1C2AE7DCD27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E12FCE51-6DB1-412D-BED4-06C2818D1567}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Sl No</t>
   </si>
@@ -75,6 +75,10 @@
   </si>
   <si>
     <t xml:space="preserve">Kode Cloud </t>
+  </si>
+  <si>
+    <t>id : Sandhyaramanipradeep@yahoo.com
+pass : Happy123!</t>
   </si>
 </sst>
 </file>
@@ -509,7 +513,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="31.81640625" customWidth="1"/>
-    <col min="3" max="3" width="26.08984375" customWidth="1"/>
+    <col min="3" max="3" width="44.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -545,12 +549,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>